<commit_message>
commit for manual testing
</commit_message>
<xml_diff>
--- a/proVidioETG/testDate/BundleProductSkew.xlsx
+++ b/proVidioETG/testDate/BundleProductSkew.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Bundle product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WOMENS-JEWELRY-BUNDLEM </t>
   </si>
   <si>
     <t xml:space="preserve">SONY-PS3-BUNDLEM</t>
@@ -41,7 +38,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -62,13 +59,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +103,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -122,11 +112,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,10 +133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -163,21 +149,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>